<commit_message>
Just a few minor changes to tests.  ie one test was labeled col,row instead of row, col
</commit_message>
<xml_diff>
--- a/configFiles/BoardLayout.xlsx
+++ b/configFiles/BoardLayout.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hunter Johnson\Documents\CSCI306\ClueGameHJRH\configFiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16386" windowHeight="8190" tabRatio="990"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,119 +26,101 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="28">
   <si>
-    <t xml:space="preserve">L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X</t>
+    <t>L</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>GL</t>
+  </si>
+  <si>
+    <t>LD</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ML</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of Doors: 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pink: Walkway adjacency test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">White: Door direction test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orange: adjacency list test, inside rooms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purple: Room exits adjacency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Green: Room entrance adjacency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Light Blue: test targets</t>
+    <t>E</t>
+  </si>
+  <si>
+    <t>EL</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>ML</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>AU</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>BU</t>
+  </si>
+  <si>
+    <t>CU</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>Number of Doors: 13</t>
+  </si>
+  <si>
+    <t>Pink: Walkway adjacency test</t>
+  </si>
+  <si>
+    <t>White: Door direction test</t>
+  </si>
+  <si>
+    <t>Orange: adjacency list test, inside rooms</t>
+  </si>
+  <si>
+    <t>Purple: Room exits adjacency</t>
+  </si>
+  <si>
+    <t>Green: Room entrance adjacency</t>
+  </si>
+  <si>
+    <t>Light Blue: test targets</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -151,7 +137,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,9 +198,15 @@
         <bgColor rgb="FF008000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66CC"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -222,121 +214,70 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyBorder="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="18">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="17">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="10" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Neutral" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in 40% - Accent1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Bad" xfId="22" builtinId="53" customBuiltin="true"/>
+  <cellStyles count="2">
+    <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -395,29 +336,309 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFFF66CC"/>
+      <color rgb="FFFF3399"/>
+      <color rgb="FFCC0099"/>
+      <color rgb="FFFF33CC"/>
+    </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:Z32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK32"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S11" activeCellId="0" sqref="S11"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col collapsed="false" hidden="false" max="25" min="1" style="1" width="3.8582995951417"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="1" width="9"/>
+    <col min="1" max="25" width="3.83984375" style="1"/>
+    <col min="26" max="1025" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -490,11 +711,11 @@
       <c r="X1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="Y1" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="Y1" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -567,11 +788,11 @@
       <c r="X2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Y2" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="Y2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -617,7 +838,7 @@
       <c r="O3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="17" t="s">
         <v>1</v>
       </c>
       <c r="Q3" s="3" t="s">
@@ -644,11 +865,11 @@
       <c r="X3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Y3" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="Y3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -721,11 +942,11 @@
       <c r="X4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Y4" s="1" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="Y4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -798,11 +1019,11 @@
       <c r="X5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Y5" s="1" t="n">
+      <c r="Y5" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -875,11 +1096,11 @@
       <c r="X6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Y6" s="1" t="n">
+      <c r="Y6" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -952,11 +1173,11 @@
       <c r="X7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Y7" s="1" t="n">
+      <c r="Y7" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
@@ -1029,11 +1250,11 @@
       <c r="X8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Y8" s="1" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="Y8" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
         <v>1</v>
       </c>
@@ -1106,14 +1327,14 @@
       <c r="X9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Y9" s="1" t="n">
+      <c r="Y9" s="1">
         <v>8</v>
       </c>
       <c r="Z9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
@@ -1186,11 +1407,11 @@
       <c r="X10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="Y10" s="1" t="n">
+      <c r="Y10" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
@@ -1263,11 +1484,11 @@
       <c r="X11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="Y11" s="1" t="n">
+      <c r="Y11" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
@@ -1340,11 +1561,11 @@
       <c r="X12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="Y12" s="1" t="n">
+      <c r="Y12" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
@@ -1417,11 +1638,11 @@
       <c r="X13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="Y13" s="1" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="Y13" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
@@ -1494,11 +1715,11 @@
       <c r="X14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="Y14" s="1" t="n">
+      <c r="Y14" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3" t="s">
         <v>1</v>
       </c>
@@ -1571,11 +1792,11 @@
       <c r="X15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="Y15" s="1" t="n">
+      <c r="Y15" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
@@ -1648,11 +1869,11 @@
       <c r="X16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="Y16" s="1" t="n">
+      <c r="Y16" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3" t="s">
         <v>1</v>
       </c>
@@ -1725,11 +1946,11 @@
       <c r="X17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="Y17" s="1" t="n">
+      <c r="Y17" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3" t="s">
         <v>1</v>
       </c>
@@ -1802,11 +2023,11 @@
       <c r="X18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="Y18" s="1" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="Y18" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3" t="s">
         <v>1</v>
       </c>
@@ -1879,11 +2100,11 @@
       <c r="X19" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="Y19" s="1" t="n">
+      <c r="Y19" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3" t="s">
         <v>1</v>
       </c>
@@ -1956,11 +2177,11 @@
       <c r="X20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="Y20" s="1" t="n">
+      <c r="Y20" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3" t="s">
         <v>1</v>
       </c>
@@ -2033,11 +2254,11 @@
       <c r="X21" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="Y21" s="1" t="n">
+      <c r="Y21" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="5" t="s">
         <v>1</v>
       </c>
@@ -2110,126 +2331,121 @@
       <c r="X22" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="Y22" s="1" t="n">
+      <c r="Y22" s="1">
         <v>21</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B23" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D23" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E23" s="1" t="n">
+    <row r="23" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="1">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3</v>
+      </c>
+      <c r="E23" s="1">
         <v>4</v>
       </c>
-      <c r="F23" s="1" t="n">
+      <c r="F23" s="1">
         <v>5</v>
       </c>
-      <c r="G23" s="1" t="n">
+      <c r="G23" s="1">
         <v>6</v>
       </c>
-      <c r="H23" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="I23" s="1" t="n">
+      <c r="H23" s="1">
+        <v>7</v>
+      </c>
+      <c r="I23" s="1">
         <v>8</v>
       </c>
-      <c r="J23" s="1" t="n">
+      <c r="J23" s="1">
         <v>9</v>
       </c>
-      <c r="K23" s="1" t="n">
+      <c r="K23" s="1">
         <v>10</v>
       </c>
-      <c r="L23" s="1" t="n">
+      <c r="L23" s="1">
         <v>11</v>
       </c>
-      <c r="M23" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="N23" s="1" t="n">
+      <c r="M23" s="1">
+        <v>12</v>
+      </c>
+      <c r="N23" s="1">
         <v>13</v>
       </c>
-      <c r="O23" s="1" t="n">
+      <c r="O23" s="1">
         <v>14</v>
       </c>
-      <c r="P23" s="1" t="n">
+      <c r="P23" s="1">
         <v>15</v>
       </c>
-      <c r="Q23" s="1" t="n">
+      <c r="Q23" s="1">
         <v>16</v>
       </c>
-      <c r="R23" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="S23" s="1" t="n">
+      <c r="R23" s="1">
+        <v>17</v>
+      </c>
+      <c r="S23" s="1">
         <v>18</v>
       </c>
-      <c r="T23" s="1" t="n">
+      <c r="T23" s="1">
         <v>19</v>
       </c>
-      <c r="U23" s="1" t="n">
+      <c r="U23" s="1">
         <v>20</v>
       </c>
-      <c r="V23" s="1" t="n">
+      <c r="V23" s="1">
         <v>21</v>
       </c>
-      <c r="W23" s="1" t="n">
+      <c r="W23" s="1">
         <v>22</v>
       </c>
-      <c r="X23" s="1" t="n">
+      <c r="X23" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="26" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="16" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>